<commit_message>
Merged carbon emissions calculation into main Jupyter file
</commit_message>
<xml_diff>
--- a/exampleoutput.xlsx
+++ b/exampleoutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhedg\Documents\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A1F8EF9-3163-452B-9375-D783F9266077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DE4324-88E5-4B3D-B6F4-8C18754C63D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BB70291E-FDBF-43DA-B2AF-4D6A1EB9F32A}"/>
+    <workbookView xWindow="-23700" yWindow="-975" windowWidth="21585" windowHeight="12765" xr2:uid="{BB70291E-FDBF-43DA-B2AF-4D6A1EB9F32A}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>charger_number</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>cost_before_rebate</t>
+  </si>
+  <si>
+    <t>optimal</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>markup</t>
+  </si>
+  <si>
+    <t>rebate_percent</t>
   </si>
 </sst>
 </file>
@@ -412,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8BB7A-4161-4255-8EBB-E3969648940D}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -426,7 +438,7 @@
     <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -445,8 +457,17 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT(B2,"c",C2,"kW")</f>
         <v>2c7.2kW</v>
@@ -466,8 +487,17 @@
       <c r="F2">
         <v>25000</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.05</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">_xlfn.CONCAT(B3,"c",C3,"kW")</f>
         <v>10c7.2kW</v>
@@ -489,8 +519,17 @@
         <f>E3*4</f>
         <v>91600</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>2c16kW</v>
@@ -511,8 +550,17 @@
         <f t="shared" ref="F4:F5" si="1">E4*4</f>
         <v>200000</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>10c16kW</v>
@@ -532,6 +580,15 @@
       <c r="F5">
         <f t="shared" si="1"/>
         <v>240000</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Factor correction in carbon emissions
</commit_message>
<xml_diff>
--- a/exampleoutput.xlsx
+++ b/exampleoutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhedg\Documents\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DE4324-88E5-4B3D-B6F4-8C18754C63D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0DAA19-D300-47B1-85EB-16FB19CDE6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23700" yWindow="-975" windowWidth="21585" windowHeight="12765" xr2:uid="{BB70291E-FDBF-43DA-B2AF-4D6A1EB9F32A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BB70291E-FDBF-43DA-B2AF-4D6A1EB9F32A}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>charger_number</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>rebate_percent</t>
+  </si>
+  <si>
+    <t>co2_reduction</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8BB7A-4161-4255-8EBB-E3969648940D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -438,7 +441,7 @@
     <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -466,8 +469,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT(B2,"c",C2,"kW")</f>
         <v>2c7.2kW</v>
@@ -496,8 +502,11 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>-8353124.7659143601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">_xlfn.CONCAT(B3,"c",C3,"kW")</f>
         <v>10c7.2kW</v>
@@ -528,8 +537,11 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>-8353124.7659143601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>2c16kW</v>
@@ -559,8 +571,11 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <v>-8353124.7659143601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>10c16kW</v>
@@ -589,6 +604,9 @@
       </c>
       <c r="I5" t="s">
         <v>9</v>
+      </c>
+      <c r="J5">
+        <v>-8353124.7659143601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>